<commit_message>
Completed profiling against demographics and produced graphs for each profile to cluster
</commit_message>
<xml_diff>
--- a/MM_PCA.xlsx
+++ b/MM_PCA.xlsx
@@ -1,21 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\OneDrive - Macquarie University\MQ_2021_S1\BUSA3020\Assessments\Assessment 3 - Clustering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mqoutlook-my.sharepoint.com/personal/cyrus_kwan_students_mq_edu_au/Documents/MQ_2021_S1/BUSA3020/Assessments/Assessment 3 - Clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5C800DB-63F5-4D7C-94B3-BB9FB97C5BC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{D5C800DB-63F5-4D7C-94B3-BB9FB97C5BC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{E82CFC6A-E413-4549-92C5-DBC1D06F9777}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Preferences_PCA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -199,9 +210,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -682,7 +693,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1037,11 +1048,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AD30"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.36328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>